<commit_message>
updated text for measurea and removed duplicates from the translations folder
</commit_message>
<xml_diff>
--- a/measures/2 master measures/text/awareness_2b.xlsx
+++ b/measures/2 master measures/text/awareness_2b.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/unconscious-ec-RRR/measures/2 master measures/text/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmoranyo\Documents\LipLab\projects\RRR_fazio&amp;olson2001\replication_procedure\OSF\measures\text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C615BD3-77FF-B84B-8B83-EC31421341C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="960" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="3000" windowWidth="26820" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,29 +30,29 @@
   </si>
   <si>
     <t>During the first task, which of the two characters was consistently presented with POSITIVE images and words? 
-1 = [CS1] (certainly)
-2 = [CS1] (probably)
-3 = [CS1] (guess)
-4 = [CS2] (guess)
-5 = [CS2] (probably)
-6 = [CS2] (certainly)
+1 = BERGMITE (certainly)
+2 = BERGMITE (probably)
+3 = BERGMITE (guess)
+4 = PALPITOAD (guess)
+5 = PALPITOAD (probably)
+6 = PALPITOAD (certainly)
 Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>During the first task, which of the two characters was consistently presented with NEGATIVE images and words? 
-1 = [CS1] (certainly)
-2 = [CS1] (probably)
-3 = [CS1] (guess)
-4 = [CS2] (guess)
-5 = [CS2] (probably)
-6 = [CS2] (certainly)
+1 = BERGMITE (certainly)
+2 = BERGMITE (probably)
+3 = BERGMITE (guess)
+4 = PALPITOAD (guess)
+5 = PALPITOAD (probably)
+6 = PALPITOAD (certainly)
 Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -651,7 +650,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -703,7 +702,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -904,29 +903,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
+    <col min="1" max="1" width="89.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="195" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="198" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>